<commit_message>
simulate selling item and generate balance sheet and income statement based on that
</commit_message>
<xml_diff>
--- a/docs/accounting/v8-v9/01_simple_purchase.xlsx
+++ b/docs/accounting/v8-v9/01_simple_purchase.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Scenario" sheetId="1" state="visible" r:id="rId2"/>
@@ -469,19 +469,19 @@
     <t xml:space="preserve">transaction_id</t>
   </si>
   <si>
-    <t xml:space="preserve">currency_debit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">currency_credit</t>
+    <t xml:space="preserve">currency_dr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">currency_cr</t>
   </si>
   <si>
     <t xml:space="preserve">currency_balance</t>
   </si>
   <si>
-    <t xml:space="preserve">debit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">credit</t>
+    <t xml:space="preserve">dr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cr</t>
   </si>
   <si>
     <t xml:space="preserve">balance</t>
@@ -513,6 +513,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">select destination and source in level of </t>
     </r>
@@ -522,6 +523,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">item</t>
     </r>
@@ -530,6 +532,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> or </t>
     </r>
@@ -539,6 +542,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">invoice</t>
     </r>
@@ -586,6 +590,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">shipping/instant</t>
     </r>
@@ -594,6 +599,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">, there is two way for inventory, the first one is locking system, which is usefull if we lock the items then transfer them as out, the other one as soon as inventory applied the inventory will saved</t>
     </r>
@@ -622,6 +628,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -643,23 +650,27 @@
       <color rgb="FF4C4C4C"/>
       <name val="DejaVu Sans"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="8"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="8"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -667,12 +678,14 @@
       <color rgb="FFED1C24"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="8"/>
       <color rgb="FFED1C24"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -801,7 +814,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1029,8 +1042,8 @@
   </sheetPr>
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A27" activeCellId="0" sqref="A27"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B27" activeCellId="0" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1449,7 +1462,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1466,22 +1479,22 @@
   <dimension ref="A1:AMJ6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F10" activeCellId="0" sqref="F10"/>
+      <selection pane="topLeft" activeCell="H3" activeCellId="0" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="27" width="5.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="14" width="13.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="14" width="13.71"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="14" width="11.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="14" width="9.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="14" width="12.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="14" width="12.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="14" width="12.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="14" width="14.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="14" width="5.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="14" width="4.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="14" width="6.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="14" width="9.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="14" width="9.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="25" width="9.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="25" width="9.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="25" width="8.79"/>
@@ -1717,7 +1730,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1820,7 +1833,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1845,8 +1858,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="33" width="11.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="33" width="28.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="34" width="11.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="35" width="39.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="33" width="9.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="35" width="39.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="33" width="9.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="33" width="9.35"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1014" min="8" style="33" width="11.52"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1015" style="36" width="11.52"/>
@@ -2050,7 +2063,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -2064,10 +2077,10 @@
     <tabColor rgb="FF00599D"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2189,13 +2202,8 @@
       <c r="F10" s="11"/>
       <c r="G10" s="12"/>
     </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="7" t="n">
-        <v>13</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="8">
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="D2:E2"/>
@@ -2204,11 +2212,10 @@
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="D7:E7"/>
     <mergeCell ref="F7:G7"/>
-    <mergeCell ref="A13:A16"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -2232,7 +2239,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="13" width="8.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="14" width="10.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="14" width="7.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="14" width="9.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="14" width="9.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="14" width="8.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="14" width="8.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="14" width="5.81"/>
@@ -2323,7 +2330,8 @@
       <c r="I3" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="J3" s="20" t="b">
+      <c r="J3" s="20" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="K3" s="21" t="s">
@@ -2365,7 +2373,8 @@
       <c r="I4" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="J4" s="20" t="b">
+      <c r="J4" s="20" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="K4" s="21" t="s">
@@ -2407,7 +2416,8 @@
       <c r="I5" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="J5" s="20" t="b">
+      <c r="J5" s="20" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="K5" s="21" t="s">
@@ -2449,7 +2459,8 @@
       <c r="I6" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="J6" s="20" t="b">
+      <c r="J6" s="20" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="K6" s="21" t="s">
@@ -2491,7 +2502,8 @@
       <c r="I7" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="J7" s="20" t="b">
+      <c r="J7" s="20" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="K7" s="21" t="s">
@@ -2533,7 +2545,8 @@
       <c r="I8" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="J8" s="23" t="b">
+      <c r="J8" s="23" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="K8" s="14" t="s">
@@ -2575,7 +2588,8 @@
       <c r="I9" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="J9" s="23" t="b">
+      <c r="J9" s="23" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="K9" s="14" t="s">
@@ -2616,7 +2630,8 @@
       <c r="I10" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="J10" s="23" t="b">
+      <c r="J10" s="23" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="K10" s="14" t="s">
@@ -2657,7 +2672,8 @@
       <c r="I11" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="J11" s="23" t="b">
+      <c r="J11" s="23" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="K11" s="14" t="s">
@@ -2698,7 +2714,8 @@
       <c r="I12" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="J12" s="23" t="b">
+      <c r="J12" s="23" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="K12" s="14" t="s">
@@ -2739,7 +2756,8 @@
       <c r="I13" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="J13" s="23" t="b">
+      <c r="J13" s="23" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="K13" s="14" t="s">
@@ -2755,7 +2773,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -2777,8 +2795,8 @@
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="13" width="8.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="14" width="12.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="14" width="9.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="14" width="12.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="14" width="9.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="15" width="8.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="14" width="8.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="14" width="13.65"/>
@@ -2846,7 +2864,8 @@
       <c r="D3" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="E3" s="23" t="b">
+      <c r="E3" s="23" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="F3" s="14" t="s">
@@ -2875,7 +2894,8 @@
       <c r="D4" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="E4" s="23" t="b">
+      <c r="E4" s="23" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="F4" s="14" t="s">
@@ -2902,7 +2922,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -2924,9 +2944,9 @@
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="13" width="8.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="14" width="12.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="14" width="9.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="15" width="9.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="14" width="12.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="14" width="9.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="15" width="9.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="15" width="8.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="14" width="8.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="14" width="13.65"/>
@@ -3035,7 +3055,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -3058,17 +3078,17 @@
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="27" width="5.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="14" width="10.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="14" width="9.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="14" width="9.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="15" width="11.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="15" width="10.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="14" width="10.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="14" width="4.48"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="14" width="9.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="14" width="9.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="14" width="5.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="25" width="7.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="25" width="12.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="25" width="14.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="14" width="9.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="14" width="9.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="14" width="9.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="14" width="9.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="14" width="8.79"/>
@@ -3180,7 +3200,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -3215,7 +3235,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="28" width="9.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="25" width="7.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="25" width="8.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="14" width="9.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="14" width="9.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="14" width="9.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="14" width="9.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="14" width="8.79"/>
@@ -3349,7 +3369,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -3372,8 +3392,8 @@
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="27" width="5.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="14" width="12.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="14" width="12.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="14" width="8.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="14" width="12.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="14" width="8.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="14" width="8.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="14" width="4.48"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="7" style="25" width="11.52"/>
@@ -3447,7 +3467,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -3473,7 +3493,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="14" width="10.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="14" width="13.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="14" width="5.32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="14" width="3.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="14" width="3.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="14" width="9.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="25" width="9.07"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="10" min="9" style="25" width="11.52"/>
@@ -3582,7 +3602,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>